<commit_message>
Excel terminé en théorie, à relire par qqn d'autre pour vérifier
</commit_message>
<xml_diff>
--- a/MetroParis.xlsx
+++ b/MetroParis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Documents\Cours_ESILV_Année_2\Pb_scientifique_info\Liv-in-Paris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4D59AE-D85E-498B-A666-4548C9D53E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB51A6D-EE17-49A7-800B-3F7217EA1FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6A7959BE-A0B4-4EB6-8342-15F77AC26B90}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="775">
   <si>
     <t>Libelle Line</t>
   </si>
@@ -2361,6 +2361,9 @@
   </si>
   <si>
     <t>Oui</t>
+  </si>
+  <si>
+    <t>Marche</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2401,6 +2404,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2414,11 +2423,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2733,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6549EE12-F9D9-4064-922E-DFCA0A3CB738}">
-  <dimension ref="A1:G333"/>
+  <dimension ref="A1:G346"/>
   <sheetViews>
-    <sheetView topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="H351" sqref="H351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10403,6 +10413,305 @@
         <v>75113</v>
       </c>
     </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>333</v>
+      </c>
+      <c r="B334" t="s">
+        <v>774</v>
+      </c>
+      <c r="C334" t="s">
+        <v>108</v>
+      </c>
+      <c r="D334" t="s">
+        <v>109</v>
+      </c>
+      <c r="E334" t="s">
+        <v>110</v>
+      </c>
+      <c r="F334" t="s">
+        <v>107</v>
+      </c>
+      <c r="G334">
+        <v>75110</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>334</v>
+      </c>
+      <c r="B335" t="s">
+        <v>774</v>
+      </c>
+      <c r="C335" t="s">
+        <v>225</v>
+      </c>
+      <c r="D335" t="s">
+        <v>226</v>
+      </c>
+      <c r="E335" t="s">
+        <v>227</v>
+      </c>
+      <c r="F335" t="s">
+        <v>107</v>
+      </c>
+      <c r="G335">
+        <v>75110</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>335</v>
+      </c>
+      <c r="B336" t="s">
+        <v>774</v>
+      </c>
+      <c r="C336" t="s">
+        <v>162</v>
+      </c>
+      <c r="D336" t="s">
+        <v>163</v>
+      </c>
+      <c r="E336" t="s">
+        <v>164</v>
+      </c>
+      <c r="F336" t="s">
+        <v>97</v>
+      </c>
+      <c r="G336">
+        <v>75109</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>336</v>
+      </c>
+      <c r="B337" t="s">
+        <v>774</v>
+      </c>
+      <c r="C337" t="s">
+        <v>159</v>
+      </c>
+      <c r="D337" t="s">
+        <v>160</v>
+      </c>
+      <c r="E337" t="s">
+        <v>161</v>
+      </c>
+      <c r="F337" t="s">
+        <v>19</v>
+      </c>
+      <c r="G337">
+        <v>75108</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>337</v>
+      </c>
+      <c r="B338" t="s">
+        <v>774</v>
+      </c>
+      <c r="C338" t="s">
+        <v>577</v>
+      </c>
+      <c r="D338" t="s">
+        <v>578</v>
+      </c>
+      <c r="E338" t="s">
+        <v>579</v>
+      </c>
+      <c r="F338" t="s">
+        <v>19</v>
+      </c>
+      <c r="G338">
+        <v>75108</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>338</v>
+      </c>
+      <c r="B339" t="s">
+        <v>774</v>
+      </c>
+      <c r="C339" t="s">
+        <v>240</v>
+      </c>
+      <c r="D339" t="s">
+        <v>241</v>
+      </c>
+      <c r="E339" t="s">
+        <v>242</v>
+      </c>
+      <c r="F339" t="s">
+        <v>32</v>
+      </c>
+      <c r="G339">
+        <v>75101</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>339</v>
+      </c>
+      <c r="B340" t="s">
+        <v>774</v>
+      </c>
+      <c r="C340" t="s">
+        <v>39</v>
+      </c>
+      <c r="D340" t="s">
+        <v>40</v>
+      </c>
+      <c r="E340" t="s">
+        <v>41</v>
+      </c>
+      <c r="F340" t="s">
+        <v>42</v>
+      </c>
+      <c r="G340">
+        <v>75104</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>340</v>
+      </c>
+      <c r="B341" t="s">
+        <v>774</v>
+      </c>
+      <c r="C341" t="s">
+        <v>228</v>
+      </c>
+      <c r="D341" t="s">
+        <v>229</v>
+      </c>
+      <c r="E341" t="s">
+        <v>230</v>
+      </c>
+      <c r="F341" t="s">
+        <v>107</v>
+      </c>
+      <c r="G341">
+        <v>75110</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>341</v>
+      </c>
+      <c r="B342" t="s">
+        <v>774</v>
+      </c>
+      <c r="C342" t="s">
+        <v>404</v>
+      </c>
+      <c r="D342" t="s">
+        <v>405</v>
+      </c>
+      <c r="E342" t="s">
+        <v>406</v>
+      </c>
+      <c r="F342" t="s">
+        <v>107</v>
+      </c>
+      <c r="G342">
+        <v>75110</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>342</v>
+      </c>
+      <c r="B343" t="s">
+        <v>774</v>
+      </c>
+      <c r="C343" t="s">
+        <v>607</v>
+      </c>
+      <c r="D343" t="s">
+        <v>608</v>
+      </c>
+      <c r="E343" t="s">
+        <v>609</v>
+      </c>
+      <c r="F343" t="s">
+        <v>312</v>
+      </c>
+      <c r="G343">
+        <v>75105</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>343</v>
+      </c>
+      <c r="B344" t="s">
+        <v>774</v>
+      </c>
+      <c r="C344" t="s">
+        <v>246</v>
+      </c>
+      <c r="D344" t="s">
+        <v>247</v>
+      </c>
+      <c r="E344" t="s">
+        <v>248</v>
+      </c>
+      <c r="F344" t="s">
+        <v>249</v>
+      </c>
+      <c r="G344">
+        <v>75106</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>344</v>
+      </c>
+      <c r="B345" t="s">
+        <v>774</v>
+      </c>
+      <c r="C345" t="s">
+        <v>165</v>
+      </c>
+      <c r="D345" t="s">
+        <v>166</v>
+      </c>
+      <c r="E345" t="s">
+        <v>167</v>
+      </c>
+      <c r="F345" t="s">
+        <v>97</v>
+      </c>
+      <c r="G345">
+        <v>75109</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>345</v>
+      </c>
+      <c r="B346" t="s">
+        <v>774</v>
+      </c>
+      <c r="C346" t="s">
+        <v>159</v>
+      </c>
+      <c r="D346" t="s">
+        <v>160</v>
+      </c>
+      <c r="E346" t="s">
+        <v>161</v>
+      </c>
+      <c r="F346" t="s">
+        <v>19</v>
+      </c>
+      <c r="G346">
+        <v>75108</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{6549EE12-F9D9-4064-922E-DFCA0A3CB738}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10411,10 +10720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CFEF04-CB9F-4D0E-AA44-E5CDB48F03B4}">
-  <dimension ref="A1:G333"/>
+  <dimension ref="A1:G346"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="D333" sqref="D333:E333"/>
+    <sheetView tabSelected="1" topLeftCell="A320" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F349" sqref="F349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10461,6 +10770,7 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
+      <c r="F2" s="1"/>
       <c r="G2" t="s">
         <v>772</v>
       </c>
@@ -10551,6 +10861,9 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
       <c r="G6" t="s">
         <v>772</v>
       </c>
@@ -10573,6 +10886,9 @@
       <c r="E7">
         <v>3</v>
       </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
       <c r="G7" t="s">
         <v>772</v>
       </c>
@@ -10595,6 +10911,9 @@
       <c r="E8">
         <v>2</v>
       </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
       <c r="G8" t="s">
         <v>772</v>
       </c>
@@ -10666,65 +10985,74 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="E12">
-        <v>2</v>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
       </c>
       <c r="G12" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>3</v>
       </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
       <c r="G13" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
         <v>2</v>
       </c>
       <c r="G14" t="s">
@@ -10749,27 +11077,33 @@
       <c r="E15">
         <v>4</v>
       </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
       <c r="G15" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="E16">
-        <v>2</v>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>4</v>
       </c>
       <c r="G16" t="s">
         <v>772</v>
@@ -10793,50 +11127,57 @@
       <c r="E17">
         <v>2</v>
       </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
       <c r="G17" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E18">
-        <v>2</v>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4</v>
       </c>
       <c r="G18" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="G19" t="s">
         <v>772</v>
       </c>
@@ -10982,20 +11323,23 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>25</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>27</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
       </c>
       <c r="G27" t="s">
         <v>772</v>
@@ -11022,19 +11366,22 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>27</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>29</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
         <v>2</v>
       </c>
       <c r="G29" t="s">
@@ -11062,19 +11409,22 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>29</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>31</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31" t="s">
@@ -11103,21 +11453,24 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <f>C32+1</f>
         <v>31</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <f t="shared" ref="D33:D43" si="2">D32+1</f>
         <v>33</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
         <v>2</v>
       </c>
       <c r="G33" t="s">
@@ -11147,44 +11500,50 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="E35">
-        <v>2</v>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>3</v>
       </c>
       <c r="G35" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="E36">
-        <v>2</v>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36" s="2">
+        <v>3</v>
       </c>
       <c r="G36" t="s">
         <v>772</v>
@@ -11213,21 +11572,24 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
         <v>2</v>
       </c>
       <c r="G38" t="s">
@@ -11279,22 +11641,25 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>1</v>
+      </c>
+      <c r="F41" s="2">
+        <v>2</v>
       </c>
       <c r="G41" t="s">
         <v>772</v>
@@ -11378,6 +11743,9 @@
       <c r="E45" s="1">
         <v>2</v>
       </c>
+      <c r="F45" s="2">
+        <v>4</v>
+      </c>
       <c r="G45" t="s">
         <v>772</v>
       </c>
@@ -11476,6 +11844,9 @@
       <c r="E50">
         <v>2</v>
       </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
       <c r="G50" t="s">
         <v>772</v>
       </c>
@@ -11516,6 +11887,9 @@
       <c r="E52">
         <v>2</v>
       </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
       <c r="G52" t="s">
         <v>772</v>
       </c>
@@ -11536,6 +11910,9 @@
       <c r="E53">
         <v>2</v>
       </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
       <c r="G53" t="s">
         <v>772</v>
       </c>
@@ -11556,6 +11933,9 @@
       <c r="E54">
         <v>2</v>
       </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
       <c r="G54" t="s">
         <v>772</v>
       </c>
@@ -11636,6 +12016,9 @@
       <c r="E58">
         <v>2</v>
       </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
       <c r="G58" t="s">
         <v>772</v>
       </c>
@@ -11656,6 +12039,9 @@
       <c r="E59">
         <v>2</v>
       </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
       <c r="G59" t="s">
         <v>772</v>
       </c>
@@ -11696,6 +12082,9 @@
       <c r="E61">
         <v>2</v>
       </c>
+      <c r="F61">
+        <v>4</v>
+      </c>
       <c r="G61" t="s">
         <v>772</v>
       </c>
@@ -11756,6 +12145,9 @@
       <c r="E64">
         <v>2</v>
       </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
       <c r="G64" t="s">
         <v>772</v>
       </c>
@@ -11776,6 +12168,9 @@
       <c r="E65">
         <v>2</v>
       </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
       <c r="G65" t="s">
         <v>772</v>
       </c>
@@ -11794,6 +12189,9 @@
       <c r="E66" s="1">
         <v>2</v>
       </c>
+      <c r="F66" s="1">
+        <v>3</v>
+      </c>
       <c r="G66" t="s">
         <v>772</v>
       </c>
@@ -11812,6 +12210,9 @@
       <c r="E67" s="1">
         <v>0</v>
       </c>
+      <c r="F67" s="1">
+        <v>3</v>
+      </c>
       <c r="G67" t="s">
         <v>772</v>
       </c>
@@ -11873,6 +12274,9 @@
       <c r="E70" s="1">
         <v>2</v>
       </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
       <c r="G70" t="s">
         <v>772</v>
       </c>
@@ -11933,6 +12337,9 @@
       <c r="E73">
         <v>2</v>
       </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
       <c r="G73" t="s">
         <v>772</v>
       </c>
@@ -11975,6 +12382,9 @@
       <c r="E75">
         <v>2</v>
       </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
       <c r="G75" t="s">
         <v>772</v>
       </c>
@@ -11996,6 +12406,9 @@
       <c r="E76">
         <v>2</v>
       </c>
+      <c r="F76">
+        <v>5</v>
+      </c>
       <c r="G76" t="s">
         <v>772</v>
       </c>
@@ -12017,6 +12430,9 @@
       <c r="E77">
         <v>2</v>
       </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
       <c r="G77" t="s">
         <v>772</v>
       </c>
@@ -12059,6 +12475,9 @@
       <c r="E79">
         <v>2</v>
       </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
       <c r="G79" t="s">
         <v>772</v>
       </c>
@@ -12080,6 +12499,9 @@
       <c r="E80">
         <v>2</v>
       </c>
+      <c r="F80">
+        <v>2</v>
+      </c>
       <c r="G80" t="s">
         <v>772</v>
       </c>
@@ -12143,6 +12565,9 @@
       <c r="E83">
         <v>2</v>
       </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
       <c r="G83" t="s">
         <v>772</v>
       </c>
@@ -12206,6 +12631,9 @@
       <c r="E86">
         <v>2</v>
       </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
       <c r="G86" t="s">
         <v>772</v>
       </c>
@@ -12290,6 +12718,9 @@
       <c r="E90">
         <v>2</v>
       </c>
+      <c r="F90">
+        <v>5</v>
+      </c>
       <c r="G90" t="s">
         <v>772</v>
       </c>
@@ -12332,6 +12763,9 @@
       <c r="E92">
         <v>2</v>
       </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
       <c r="G92" t="s">
         <v>772</v>
       </c>
@@ -12352,6 +12786,9 @@
       </c>
       <c r="E93">
         <v>2</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
       </c>
       <c r="G93" t="s">
         <v>772</v>
@@ -12499,6 +12936,9 @@
       <c r="E100">
         <v>2</v>
       </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
       <c r="G100" t="s">
         <v>772</v>
       </c>
@@ -12521,6 +12961,9 @@
       <c r="E101">
         <v>2</v>
       </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
       <c r="G101" t="s">
         <v>772</v>
       </c>
@@ -12543,6 +12986,9 @@
       <c r="E102">
         <v>2</v>
       </c>
+      <c r="F102">
+        <v>5</v>
+      </c>
       <c r="G102" t="s">
         <v>772</v>
       </c>
@@ -12565,6 +13011,9 @@
       <c r="E103">
         <v>2</v>
       </c>
+      <c r="F103">
+        <v>5</v>
+      </c>
       <c r="G103" t="s">
         <v>772</v>
       </c>
@@ -12609,6 +13058,9 @@
       <c r="E105">
         <v>2</v>
       </c>
+      <c r="F105">
+        <v>4</v>
+      </c>
       <c r="G105" t="s">
         <v>772</v>
       </c>
@@ -12631,6 +13083,9 @@
       <c r="E106">
         <v>2</v>
       </c>
+      <c r="F106">
+        <v>2</v>
+      </c>
       <c r="G106" t="s">
         <v>772</v>
       </c>
@@ -12697,6 +13152,9 @@
       <c r="E109">
         <v>2</v>
       </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
       <c r="G109" t="s">
         <v>772</v>
       </c>
@@ -12741,6 +13199,9 @@
       <c r="E111">
         <v>2</v>
       </c>
+      <c r="F111">
+        <v>4</v>
+      </c>
       <c r="G111" t="s">
         <v>772</v>
       </c>
@@ -12803,6 +13264,9 @@
       <c r="D114" s="1"/>
       <c r="E114" s="1">
         <v>2</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
       </c>
       <c r="G114" t="s">
         <v>772</v>
@@ -12823,6 +13287,9 @@
       <c r="E115" s="1">
         <v>0</v>
       </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
       <c r="G115" t="s">
         <v>772</v>
       </c>
@@ -12889,6 +13356,9 @@
       <c r="E118">
         <v>2</v>
       </c>
+      <c r="F118">
+        <v>2</v>
+      </c>
       <c r="G118" t="s">
         <v>772</v>
       </c>
@@ -12977,6 +13447,9 @@
       <c r="E122">
         <v>2</v>
       </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
       <c r="G122" t="s">
         <v>772</v>
       </c>
@@ -13043,6 +13516,9 @@
       <c r="E125">
         <v>2</v>
       </c>
+      <c r="F125">
+        <v>2</v>
+      </c>
       <c r="G125" t="s">
         <v>772</v>
       </c>
@@ -13065,6 +13541,9 @@
       <c r="E126">
         <v>2</v>
       </c>
+      <c r="F126">
+        <v>5</v>
+      </c>
       <c r="G126" t="s">
         <v>772</v>
       </c>
@@ -13109,6 +13588,9 @@
       <c r="E128">
         <v>2</v>
       </c>
+      <c r="F128">
+        <v>2</v>
+      </c>
       <c r="G128" t="s">
         <v>772</v>
       </c>
@@ -13131,6 +13613,9 @@
       <c r="E129">
         <v>2</v>
       </c>
+      <c r="F129">
+        <v>3</v>
+      </c>
       <c r="G129" t="s">
         <v>772</v>
       </c>
@@ -13219,6 +13704,9 @@
       <c r="E133">
         <v>2</v>
       </c>
+      <c r="F133">
+        <v>3</v>
+      </c>
       <c r="G133" t="s">
         <v>772</v>
       </c>
@@ -13307,6 +13795,9 @@
       <c r="E137">
         <v>2</v>
       </c>
+      <c r="F137">
+        <v>4</v>
+      </c>
       <c r="G137" t="s">
         <v>772</v>
       </c>
@@ -13351,6 +13842,9 @@
       <c r="E139">
         <v>2</v>
       </c>
+      <c r="F139">
+        <v>2</v>
+      </c>
       <c r="G139" t="s">
         <v>772</v>
       </c>
@@ -13413,6 +13907,9 @@
       <c r="D142" s="1"/>
       <c r="E142" s="1">
         <v>2</v>
+      </c>
+      <c r="F142">
+        <v>4</v>
       </c>
       <c r="G142" t="s">
         <v>772</v>
@@ -13521,6 +14018,9 @@
       <c r="E147">
         <v>2</v>
       </c>
+      <c r="F147">
+        <v>3</v>
+      </c>
       <c r="G147" t="s">
         <v>772</v>
       </c>
@@ -13543,6 +14043,9 @@
       <c r="E148">
         <v>2</v>
       </c>
+      <c r="F148">
+        <v>2</v>
+      </c>
       <c r="G148" t="s">
         <v>772</v>
       </c>
@@ -13587,6 +14090,9 @@
       <c r="E150">
         <v>2</v>
       </c>
+      <c r="F150">
+        <v>5</v>
+      </c>
       <c r="G150" t="s">
         <v>772</v>
       </c>
@@ -13675,6 +14181,9 @@
       <c r="E154">
         <v>2</v>
       </c>
+      <c r="F154">
+        <v>2</v>
+      </c>
       <c r="G154" t="s">
         <v>772</v>
       </c>
@@ -13697,6 +14206,9 @@
       <c r="E155">
         <v>2</v>
       </c>
+      <c r="F155">
+        <v>3</v>
+      </c>
       <c r="G155" t="s">
         <v>772</v>
       </c>
@@ -13719,6 +14231,9 @@
       <c r="E156">
         <v>2</v>
       </c>
+      <c r="F156">
+        <v>2</v>
+      </c>
       <c r="G156" t="s">
         <v>772</v>
       </c>
@@ -13741,6 +14256,9 @@
       <c r="E157">
         <v>2</v>
       </c>
+      <c r="F157">
+        <v>2</v>
+      </c>
       <c r="G157" t="s">
         <v>772</v>
       </c>
@@ -13785,6 +14303,9 @@
       <c r="E159">
         <v>2</v>
       </c>
+      <c r="F159">
+        <v>5</v>
+      </c>
       <c r="G159" t="s">
         <v>772</v>
       </c>
@@ -13851,6 +14372,9 @@
       <c r="E162">
         <v>2</v>
       </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
       <c r="G162" t="s">
         <v>772</v>
       </c>
@@ -13939,6 +14463,9 @@
       <c r="E166">
         <v>2</v>
       </c>
+      <c r="F166">
+        <v>3</v>
+      </c>
       <c r="G166" t="s">
         <v>772</v>
       </c>
@@ -13983,6 +14510,9 @@
       <c r="E168">
         <v>2</v>
       </c>
+      <c r="F168">
+        <v>1</v>
+      </c>
       <c r="G168" t="s">
         <v>772</v>
       </c>
@@ -14064,6 +14594,9 @@
       <c r="D172" s="1"/>
       <c r="E172" s="1">
         <v>2</v>
+      </c>
+      <c r="F172">
+        <v>1</v>
       </c>
       <c r="G172" t="s">
         <v>772</v>
@@ -14084,6 +14617,9 @@
       <c r="E173" s="1">
         <v>0</v>
       </c>
+      <c r="F173">
+        <v>2</v>
+      </c>
       <c r="G173" t="s">
         <v>772</v>
       </c>
@@ -14106,6 +14642,9 @@
       <c r="E174">
         <v>2</v>
       </c>
+      <c r="F174">
+        <v>3</v>
+      </c>
       <c r="G174" t="s">
         <v>772</v>
       </c>
@@ -14172,6 +14711,9 @@
       <c r="E177">
         <v>2</v>
       </c>
+      <c r="F177">
+        <v>1</v>
+      </c>
       <c r="G177" t="s">
         <v>773</v>
       </c>
@@ -14194,6 +14736,9 @@
       <c r="E178">
         <v>2</v>
       </c>
+      <c r="F178">
+        <v>2</v>
+      </c>
       <c r="G178" t="s">
         <v>773</v>
       </c>
@@ -14256,6 +14801,9 @@
       <c r="D181" s="3"/>
       <c r="E181">
         <v>2</v>
+      </c>
+      <c r="F181">
+        <v>1</v>
       </c>
       <c r="G181" t="s">
         <v>773</v>
@@ -14386,6 +14934,9 @@
       <c r="E187">
         <v>2</v>
       </c>
+      <c r="F187">
+        <v>3</v>
+      </c>
       <c r="G187" t="s">
         <v>772</v>
       </c>
@@ -14452,6 +15003,9 @@
       <c r="E190">
         <v>2</v>
       </c>
+      <c r="F190">
+        <v>3</v>
+      </c>
       <c r="G190" t="s">
         <v>772</v>
       </c>
@@ -14474,6 +15028,9 @@
       <c r="E191">
         <v>2</v>
       </c>
+      <c r="F191">
+        <v>4</v>
+      </c>
       <c r="G191" t="s">
         <v>772</v>
       </c>
@@ -14496,6 +15053,9 @@
       <c r="E192">
         <v>2</v>
       </c>
+      <c r="F192">
+        <v>4</v>
+      </c>
       <c r="G192" t="s">
         <v>772</v>
       </c>
@@ -14518,6 +15078,9 @@
       <c r="E193">
         <v>2</v>
       </c>
+      <c r="F193">
+        <v>3</v>
+      </c>
       <c r="G193" t="s">
         <v>772</v>
       </c>
@@ -14540,6 +15103,9 @@
       <c r="E194">
         <v>2</v>
       </c>
+      <c r="F194">
+        <v>2</v>
+      </c>
       <c r="G194" t="s">
         <v>772</v>
       </c>
@@ -14562,6 +15128,9 @@
       <c r="E195">
         <v>2</v>
       </c>
+      <c r="F195">
+        <v>2</v>
+      </c>
       <c r="G195" t="s">
         <v>772</v>
       </c>
@@ -14584,6 +15153,9 @@
       <c r="E196">
         <v>2</v>
       </c>
+      <c r="F196">
+        <v>2</v>
+      </c>
       <c r="G196" t="s">
         <v>772</v>
       </c>
@@ -14606,6 +15178,9 @@
       <c r="E197">
         <v>2</v>
       </c>
+      <c r="F197">
+        <v>3</v>
+      </c>
       <c r="G197" t="s">
         <v>772</v>
       </c>
@@ -14628,6 +15203,9 @@
       <c r="E198">
         <v>2</v>
       </c>
+      <c r="F198">
+        <v>4</v>
+      </c>
       <c r="G198" t="s">
         <v>772</v>
       </c>
@@ -14716,6 +15294,9 @@
       <c r="E202">
         <v>2</v>
       </c>
+      <c r="F202">
+        <v>3</v>
+      </c>
       <c r="G202" t="s">
         <v>772</v>
       </c>
@@ -14782,6 +15363,9 @@
       <c r="E205">
         <v>2</v>
       </c>
+      <c r="F205">
+        <v>2</v>
+      </c>
       <c r="G205" t="s">
         <v>772</v>
       </c>
@@ -14824,6 +15408,9 @@
         <v>207</v>
       </c>
       <c r="E207">
+        <v>2</v>
+      </c>
+      <c r="F207">
         <v>2</v>
       </c>
       <c r="G207" t="s">
@@ -14951,6 +15538,9 @@
       <c r="E213">
         <v>2</v>
       </c>
+      <c r="F213">
+        <v>2</v>
+      </c>
       <c r="G213" t="s">
         <v>772</v>
       </c>
@@ -14973,6 +15563,9 @@
       <c r="E214">
         <v>2</v>
       </c>
+      <c r="F214">
+        <v>2</v>
+      </c>
       <c r="G214" t="s">
         <v>772</v>
       </c>
@@ -15083,6 +15676,9 @@
       <c r="E219">
         <v>2</v>
       </c>
+      <c r="F219">
+        <v>2</v>
+      </c>
       <c r="G219" t="s">
         <v>772</v>
       </c>
@@ -15149,6 +15745,9 @@
       <c r="E222">
         <v>2</v>
       </c>
+      <c r="F222">
+        <v>2</v>
+      </c>
       <c r="G222" t="s">
         <v>772</v>
       </c>
@@ -15193,6 +15792,9 @@
       <c r="E224">
         <v>2</v>
       </c>
+      <c r="F224">
+        <v>3</v>
+      </c>
       <c r="G224" t="s">
         <v>772</v>
       </c>
@@ -15237,6 +15839,9 @@
       <c r="E226">
         <v>2</v>
       </c>
+      <c r="F226">
+        <v>2</v>
+      </c>
       <c r="G226" t="s">
         <v>772</v>
       </c>
@@ -15259,6 +15864,9 @@
       <c r="E227">
         <v>2</v>
       </c>
+      <c r="F227">
+        <v>3</v>
+      </c>
       <c r="G227" t="s">
         <v>772</v>
       </c>
@@ -15281,6 +15889,9 @@
       <c r="E228">
         <v>2</v>
       </c>
+      <c r="F228">
+        <v>2</v>
+      </c>
       <c r="G228" t="s">
         <v>772</v>
       </c>
@@ -15303,6 +15914,9 @@
       <c r="E229">
         <v>2</v>
       </c>
+      <c r="F229">
+        <v>2</v>
+      </c>
       <c r="G229" t="s">
         <v>772</v>
       </c>
@@ -15325,6 +15939,9 @@
       <c r="E230">
         <v>2</v>
       </c>
+      <c r="F230">
+        <v>2</v>
+      </c>
       <c r="G230" t="s">
         <v>772</v>
       </c>
@@ -15347,6 +15964,9 @@
       <c r="E231">
         <v>2</v>
       </c>
+      <c r="F231">
+        <v>3</v>
+      </c>
       <c r="G231" t="s">
         <v>772</v>
       </c>
@@ -15369,6 +15989,9 @@
       <c r="E232">
         <v>2</v>
       </c>
+      <c r="F232">
+        <v>4</v>
+      </c>
       <c r="G232" t="s">
         <v>772</v>
       </c>
@@ -15391,6 +16014,9 @@
       <c r="E233">
         <v>2</v>
       </c>
+      <c r="F233">
+        <v>2</v>
+      </c>
       <c r="G233" t="s">
         <v>772</v>
       </c>
@@ -15501,6 +16127,9 @@
       <c r="E238">
         <v>2</v>
       </c>
+      <c r="F238">
+        <v>4</v>
+      </c>
       <c r="G238" t="s">
         <v>772</v>
       </c>
@@ -15582,6 +16211,9 @@
       <c r="E242" s="1">
         <v>0</v>
       </c>
+      <c r="F242" s="1">
+        <v>4</v>
+      </c>
       <c r="G242" t="s">
         <v>772</v>
       </c>
@@ -15604,6 +16236,9 @@
       <c r="E243">
         <v>2</v>
       </c>
+      <c r="F243">
+        <v>2</v>
+      </c>
       <c r="G243" t="s">
         <v>772</v>
       </c>
@@ -15692,6 +16327,9 @@
       <c r="E247">
         <v>2</v>
       </c>
+      <c r="F247">
+        <v>2</v>
+      </c>
       <c r="G247" t="s">
         <v>772</v>
       </c>
@@ -15736,6 +16374,9 @@
       <c r="E249">
         <v>2</v>
       </c>
+      <c r="F249">
+        <v>2</v>
+      </c>
       <c r="G249" t="s">
         <v>772</v>
       </c>
@@ -15780,6 +16421,9 @@
       <c r="E251">
         <v>2</v>
       </c>
+      <c r="F251">
+        <v>2</v>
+      </c>
       <c r="G251" t="s">
         <v>772</v>
       </c>
@@ -15824,6 +16468,9 @@
       <c r="E253">
         <v>2</v>
       </c>
+      <c r="F253">
+        <v>3</v>
+      </c>
       <c r="G253" t="s">
         <v>772</v>
       </c>
@@ -15932,6 +16579,9 @@
         <v>258</v>
       </c>
       <c r="E258">
+        <v>2</v>
+      </c>
+      <c r="F258">
         <v>2</v>
       </c>
       <c r="G258" t="s">
@@ -15972,6 +16622,9 @@
       <c r="E260">
         <v>0</v>
       </c>
+      <c r="F260">
+        <v>2</v>
+      </c>
       <c r="G260" t="s">
         <v>773</v>
       </c>
@@ -16035,6 +16688,9 @@
       <c r="E263" s="1">
         <v>0</v>
       </c>
+      <c r="F263">
+        <v>5</v>
+      </c>
       <c r="G263" t="s">
         <v>772</v>
       </c>
@@ -16056,6 +16712,9 @@
       <c r="E264">
         <v>2</v>
       </c>
+      <c r="F264">
+        <v>2</v>
+      </c>
       <c r="G264" t="s">
         <v>772</v>
       </c>
@@ -16100,6 +16759,9 @@
       <c r="E266">
         <v>2</v>
       </c>
+      <c r="F266">
+        <v>2</v>
+      </c>
       <c r="G266" t="s">
         <v>772</v>
       </c>
@@ -16122,6 +16784,9 @@
       <c r="E267">
         <v>2</v>
       </c>
+      <c r="F267">
+        <v>4</v>
+      </c>
       <c r="G267" t="s">
         <v>772</v>
       </c>
@@ -16166,6 +16831,9 @@
       <c r="E269">
         <v>2</v>
       </c>
+      <c r="F269">
+        <v>2</v>
+      </c>
       <c r="G269" t="s">
         <v>772</v>
       </c>
@@ -16232,6 +16900,9 @@
       <c r="E272">
         <v>2</v>
       </c>
+      <c r="F272">
+        <v>2</v>
+      </c>
       <c r="G272" t="s">
         <v>772</v>
       </c>
@@ -16272,6 +16943,9 @@
       <c r="D274" s="1"/>
       <c r="E274" s="1">
         <v>2</v>
+      </c>
+      <c r="F274">
+        <v>3</v>
       </c>
       <c r="G274" t="s">
         <v>772</v>
@@ -16336,6 +17010,9 @@
       <c r="E277">
         <v>2</v>
       </c>
+      <c r="F277">
+        <v>2</v>
+      </c>
       <c r="G277" t="s">
         <v>772</v>
       </c>
@@ -16424,6 +17101,9 @@
       <c r="E281">
         <v>2</v>
       </c>
+      <c r="F281">
+        <v>2</v>
+      </c>
       <c r="G281" t="s">
         <v>772</v>
       </c>
@@ -16512,6 +17192,9 @@
       <c r="E285">
         <v>2</v>
       </c>
+      <c r="F285">
+        <v>4</v>
+      </c>
       <c r="G285" t="s">
         <v>772</v>
       </c>
@@ -16534,6 +17217,9 @@
       <c r="E286">
         <v>2</v>
       </c>
+      <c r="F286">
+        <v>4</v>
+      </c>
       <c r="G286" t="s">
         <v>772</v>
       </c>
@@ -16556,6 +17242,9 @@
       <c r="E287">
         <v>2</v>
       </c>
+      <c r="F287">
+        <v>4</v>
+      </c>
       <c r="G287" t="s">
         <v>772</v>
       </c>
@@ -16644,6 +17333,9 @@
       <c r="E291">
         <v>2</v>
       </c>
+      <c r="F291">
+        <v>2</v>
+      </c>
       <c r="G291" t="s">
         <v>772</v>
       </c>
@@ -16710,6 +17402,9 @@
       <c r="E294">
         <v>2</v>
       </c>
+      <c r="F294">
+        <v>5</v>
+      </c>
       <c r="G294" t="s">
         <v>772</v>
       </c>
@@ -16752,6 +17447,9 @@
         <v>296</v>
       </c>
       <c r="E296">
+        <v>2</v>
+      </c>
+      <c r="F296">
         <v>2</v>
       </c>
       <c r="G296" t="s">
@@ -16946,6 +17644,9 @@
       <c r="E305">
         <v>2</v>
       </c>
+      <c r="F305">
+        <v>5</v>
+      </c>
       <c r="G305" t="s">
         <v>772</v>
       </c>
@@ -16968,6 +17669,9 @@
       <c r="E306">
         <v>2</v>
       </c>
+      <c r="F306">
+        <v>2</v>
+      </c>
       <c r="G306" t="s">
         <v>772</v>
       </c>
@@ -17034,6 +17738,9 @@
       <c r="E309">
         <v>2</v>
       </c>
+      <c r="F309">
+        <v>3</v>
+      </c>
       <c r="G309" t="s">
         <v>772</v>
       </c>
@@ -17056,6 +17763,9 @@
       <c r="E310">
         <v>2</v>
       </c>
+      <c r="F310">
+        <v>2</v>
+      </c>
       <c r="G310" t="s">
         <v>772</v>
       </c>
@@ -17078,6 +17788,9 @@
       <c r="E311">
         <v>2</v>
       </c>
+      <c r="F311">
+        <v>3</v>
+      </c>
       <c r="G311" t="s">
         <v>772</v>
       </c>
@@ -17100,6 +17813,9 @@
       <c r="E312">
         <v>2</v>
       </c>
+      <c r="F312">
+        <v>4</v>
+      </c>
       <c r="G312" t="s">
         <v>772</v>
       </c>
@@ -17144,6 +17860,9 @@
       <c r="E314">
         <v>2</v>
       </c>
+      <c r="F314">
+        <v>2</v>
+      </c>
       <c r="G314" t="s">
         <v>772</v>
       </c>
@@ -17166,6 +17885,9 @@
       <c r="E315">
         <v>2</v>
       </c>
+      <c r="F315">
+        <v>1</v>
+      </c>
       <c r="G315" t="s">
         <v>772</v>
       </c>
@@ -17229,6 +17951,9 @@
       <c r="E318">
         <v>2</v>
       </c>
+      <c r="F318">
+        <v>1</v>
+      </c>
       <c r="G318" t="s">
         <v>772</v>
       </c>
@@ -17270,6 +17995,9 @@
       <c r="E320" s="1">
         <v>2</v>
       </c>
+      <c r="F320">
+        <v>3</v>
+      </c>
       <c r="G320" t="s">
         <v>772</v>
       </c>
@@ -17288,6 +18016,9 @@
       <c r="E321" s="1">
         <v>0</v>
       </c>
+      <c r="F321" s="1">
+        <v>3</v>
+      </c>
       <c r="G321" t="s">
         <v>772</v>
       </c>
@@ -17332,6 +18063,9 @@
       <c r="E323">
         <v>2</v>
       </c>
+      <c r="F323">
+        <v>4</v>
+      </c>
       <c r="G323" t="s">
         <v>772</v>
       </c>
@@ -17354,6 +18088,9 @@
       <c r="E324">
         <v>2</v>
       </c>
+      <c r="F324">
+        <v>4</v>
+      </c>
       <c r="G324" t="s">
         <v>772</v>
       </c>
@@ -17376,6 +18113,9 @@
       <c r="E325">
         <v>2</v>
       </c>
+      <c r="F325">
+        <v>2</v>
+      </c>
       <c r="G325" t="s">
         <v>772</v>
       </c>
@@ -17398,6 +18138,9 @@
       <c r="E326">
         <v>2</v>
       </c>
+      <c r="F326">
+        <v>5</v>
+      </c>
       <c r="G326" t="s">
         <v>772</v>
       </c>
@@ -17420,6 +18163,9 @@
       <c r="E327">
         <v>2</v>
       </c>
+      <c r="F327">
+        <v>4</v>
+      </c>
       <c r="G327" t="s">
         <v>772</v>
       </c>
@@ -17442,6 +18188,9 @@
       <c r="E328">
         <v>2</v>
       </c>
+      <c r="F328">
+        <v>4</v>
+      </c>
       <c r="G328" t="s">
         <v>772</v>
       </c>
@@ -17550,6 +18299,251 @@
         <v>2</v>
       </c>
       <c r="G333" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>333</v>
+      </c>
+      <c r="B334" t="s">
+        <v>108</v>
+      </c>
+      <c r="D334">
+        <v>334</v>
+      </c>
+      <c r="E334">
+        <v>0</v>
+      </c>
+      <c r="G334" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>334</v>
+      </c>
+      <c r="B335" t="s">
+        <v>225</v>
+      </c>
+      <c r="C335">
+        <v>333</v>
+      </c>
+      <c r="E335">
+        <v>6</v>
+      </c>
+      <c r="F335">
+        <v>5</v>
+      </c>
+      <c r="G335" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>335</v>
+      </c>
+      <c r="B336" t="s">
+        <v>162</v>
+      </c>
+      <c r="D336">
+        <v>336</v>
+      </c>
+      <c r="E336">
+        <v>0</v>
+      </c>
+      <c r="F336">
+        <v>2</v>
+      </c>
+      <c r="G336" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>336</v>
+      </c>
+      <c r="B337" t="s">
+        <v>159</v>
+      </c>
+      <c r="C337">
+        <v>335</v>
+      </c>
+      <c r="D337">
+        <v>337</v>
+      </c>
+      <c r="E337">
+        <v>6</v>
+      </c>
+      <c r="F337">
+        <v>4</v>
+      </c>
+      <c r="G337" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>337</v>
+      </c>
+      <c r="B338" t="s">
+        <v>577</v>
+      </c>
+      <c r="C338">
+        <v>336</v>
+      </c>
+      <c r="E338">
+        <v>6</v>
+      </c>
+      <c r="G338" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>338</v>
+      </c>
+      <c r="B339" t="s">
+        <v>240</v>
+      </c>
+      <c r="D339">
+        <v>339</v>
+      </c>
+      <c r="E339">
+        <v>0</v>
+      </c>
+      <c r="G339" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>339</v>
+      </c>
+      <c r="B340" t="s">
+        <v>39</v>
+      </c>
+      <c r="C340">
+        <v>338</v>
+      </c>
+      <c r="E340">
+        <v>6</v>
+      </c>
+      <c r="F340">
+        <v>5</v>
+      </c>
+      <c r="G340" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>340</v>
+      </c>
+      <c r="B341" t="s">
+        <v>228</v>
+      </c>
+      <c r="D341">
+        <v>341</v>
+      </c>
+      <c r="E341">
+        <v>0</v>
+      </c>
+      <c r="F341">
+        <v>5</v>
+      </c>
+      <c r="G341" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>341</v>
+      </c>
+      <c r="B342" t="s">
+        <v>404</v>
+      </c>
+      <c r="C342">
+        <v>340</v>
+      </c>
+      <c r="E342">
+        <v>6</v>
+      </c>
+      <c r="G342" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>342</v>
+      </c>
+      <c r="B343" t="s">
+        <v>607</v>
+      </c>
+      <c r="D343">
+        <v>343</v>
+      </c>
+      <c r="E343">
+        <v>0</v>
+      </c>
+      <c r="G343" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>343</v>
+      </c>
+      <c r="B344" t="s">
+        <v>246</v>
+      </c>
+      <c r="C344">
+        <v>342</v>
+      </c>
+      <c r="E344">
+        <v>6</v>
+      </c>
+      <c r="G344" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>344</v>
+      </c>
+      <c r="B345" t="s">
+        <v>165</v>
+      </c>
+      <c r="D345">
+        <v>344</v>
+      </c>
+      <c r="E345">
+        <v>0</v>
+      </c>
+      <c r="F345">
+        <v>3</v>
+      </c>
+      <c r="G345" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>345</v>
+      </c>
+      <c r="B346" t="s">
+        <v>159</v>
+      </c>
+      <c r="C346">
+        <v>345</v>
+      </c>
+      <c r="E346">
+        <v>6</v>
+      </c>
+      <c r="F346">
+        <v>4</v>
+      </c>
+      <c r="G346" t="s">
         <v>772</v>
       </c>
     </row>

</xml_diff>